<commit_message>
Ajusta na calculadora de IPCA
</commit_message>
<xml_diff>
--- a/investimentos.xlsx
+++ b/investimentos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yukak\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yukak\Documents\wally documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B88CE1-024A-43D3-98F9-5FAAA87E3E1E}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2EBED04-C547-4186-96C6-8A32FB8E9C9D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{6D7E0E0C-83E2-46F4-9BD9-2B2078C1BDA3}"/>
   </bookViews>
@@ -20,12 +20,17 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="30">
   <si>
     <t>MAXIMA</t>
   </si>
@@ -126,7 +131,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="dd&quot;/&quot;mm&quot;/&quot;yyyy"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -160,6 +165,11 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -184,7 +194,7 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -195,6 +205,12 @@
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Moeda" xfId="1" builtinId="4"/>
@@ -512,10 +528,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA95EFB2-2EC8-48A7-BA81-301C917D56B4}">
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:XFD31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1400,6 +1416,96 @@
         <v>1000</v>
       </c>
     </row>
+    <row r="31" spans="1:9" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" s="10">
+        <f t="shared" ref="B31:B33" ca="1" si="0">YEAR(IF(C31="Liq. Diária", NOW(), C31))</f>
+        <v>2026</v>
+      </c>
+      <c r="C31" s="11">
+        <v>46059</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F31" s="12">
+        <v>0.10920000000000001</v>
+      </c>
+      <c r="G31" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="H31" s="11">
+        <v>43539</v>
+      </c>
+      <c r="I31" s="13">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" s="10">
+        <f t="shared" ca="1" si="0"/>
+        <v>2027</v>
+      </c>
+      <c r="C32" s="11">
+        <v>46479</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F32" s="12">
+        <v>0.11310000000000001</v>
+      </c>
+      <c r="G32" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="H32" s="11">
+        <v>43559</v>
+      </c>
+      <c r="I32" s="13">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" s="10">
+        <f t="shared" ca="1" si="0"/>
+        <v>2022</v>
+      </c>
+      <c r="C33" s="11">
+        <v>44697</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F33" s="12">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="G33" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="H33" s="11">
+        <v>43601</v>
+      </c>
+      <c r="I33" s="13">
+        <v>3000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>